<commit_message>
clean code, bre, msgbox
</commit_message>
<xml_diff>
--- a/betacom/working/input/Input.xlsx
+++ b/betacom/working/input/Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ja\moje\moje\uipath\betacom\zadanierekrutacyjnebetacoms_a_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ja\moje\moje\uipath\betacom\working\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2EE7A0-A151-4E3A-9567-12AC1F2B65A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA63DF-0A92-45F3-85F4-F608D8D1CE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CB34D68-E816-480A-B3B3-92DF85DBED46}"/>
   </bookViews>
@@ -77,16 +77,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>0000142065</t>
-  </si>
-  <si>
-    <t>0000419268</t>
-  </si>
-  <si>
     <t>0000951450</t>
   </si>
   <si>
     <t>00012348</t>
+  </si>
+  <si>
+    <t>0000142</t>
+  </si>
+  <si>
+    <t>00004</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -578,7 +578,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -593,7 +593,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -608,7 +608,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -735,6 +735,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DF56AAC514FF894DB9025FD6D51E167D" ma:contentTypeVersion="16" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="76c5b999bb60df58f39d3ae47f0f9a96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="915a8f8f-5e2c-47da-8ee4-e234318d0641" xmlns:ns3="5231f521-4a98-41f3-9ae1-201dce3e5a7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ab3f6e8c38bc0e4d7f7f5c8ce3e5b20" ns2:_="" ns3:_="">
     <xsd:import namespace="915a8f8f-5e2c-47da-8ee4-e234318d0641"/>
@@ -977,16 +986,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEED3417-EC0C-413E-B574-9C949658887B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{854C0DD1-8E0D-446E-A0E0-182905A1CBA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1003,12 +1011,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEED3417-EC0C-413E-B574-9C949658887B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>